<commit_message>
Ultima actualizacion a fecha 19 de marzo lo q hice hoy
</commit_message>
<xml_diff>
--- a/Cronograma-July-Tesis.xlsx
+++ b/Cronograma-July-Tesis.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="60">
   <si>
     <t>Cronograma</t>
   </si>
@@ -192,6 +192,18 @@
   </si>
   <si>
     <t>Falta corregir porque Alejo no los ha revisado :)</t>
+  </si>
+  <si>
+    <t>Falta revisar por Giovany</t>
+  </si>
+  <si>
+    <t>Falta revisar por Giovany y REFERENCIAR LA PARTE QUE DICE QUE EL CUIDADOR MUERE PRIMERO QUE EL PACIENTE</t>
+  </si>
+  <si>
+    <t>Revisar nuevamente</t>
+  </si>
+  <si>
+    <t>añadir los objetivos que faltan</t>
   </si>
 </sst>
 </file>
@@ -614,75 +626,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -690,6 +633,75 @@
       <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -974,8 +986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:C21"/>
+    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -990,10 +1002,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="24"/>
+      <c r="D2" s="19"/>
     </row>
     <row r="3" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1003,26 +1015,26 @@
       <c r="D4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="31"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="26"/>
     </row>
     <row r="5" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="32" t="s">
+      <c r="D5" s="21"/>
+      <c r="E5" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="34"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="29"/>
     </row>
     <row r="6" spans="3:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="5" t="s">
@@ -1031,13 +1043,13 @@
       <c r="D6" s="6">
         <v>0.85</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="14"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="18"/>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
@@ -1046,11 +1058,11 @@
       <c r="D7" s="4">
         <v>0</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="14"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="18"/>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
@@ -1059,13 +1071,13 @@
       <c r="D8" s="4">
         <v>0.9</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="14"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="18"/>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
@@ -1074,11 +1086,11 @@
       <c r="D9" s="4">
         <v>0</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="14"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="18"/>
     </row>
     <row r="10" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="7" t="s">
@@ -1088,102 +1100,114 @@
         <f>(D9+D8+D7+D6)/4</f>
         <v>0.4375</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="23"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="33"/>
     </row>
     <row r="11" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="15" t="s">
+      <c r="D11" s="21"/>
+      <c r="E11" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="17"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="36"/>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C12" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="6">
-        <v>0</v>
-      </c>
-      <c r="E12" s="18"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="20"/>
-    </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
+        <v>0.9</v>
+      </c>
+      <c r="E12" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="39"/>
+    </row>
+    <row r="13" spans="3:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="4">
-        <v>0</v>
-      </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="14"/>
+      <c r="D13" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="E13" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="39"/>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="4">
-        <v>0</v>
-      </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="14"/>
+        <v>0.9</v>
+      </c>
+      <c r="E14" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="39"/>
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="4">
-        <v>0</v>
-      </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="14"/>
+        <v>0.9</v>
+      </c>
+      <c r="E15" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="39"/>
     </row>
     <row r="16" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="4">
-        <v>0</v>
-      </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="14"/>
+        <v>0.5</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="18"/>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="4">
-        <v>0</v>
-      </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="14"/>
+        <v>0.4</v>
+      </c>
+      <c r="E17" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="18"/>
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
@@ -1192,11 +1216,11 @@
       <c r="D18" s="4">
         <v>0</v>
       </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="14"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="18"/>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
@@ -1205,11 +1229,11 @@
       <c r="D19" s="4">
         <v>0</v>
       </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="14"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="18"/>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C20" s="2" t="s">
@@ -1218,11 +1242,11 @@
       <c r="D20" s="4">
         <v>0</v>
       </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="14"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="18"/>
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C21" s="2" t="s">
@@ -1231,11 +1255,11 @@
       <c r="D21" s="4">
         <v>0</v>
       </c>
-      <c r="E21" s="12"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="14"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="18"/>
     </row>
     <row r="22" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C22" s="2" t="s">
@@ -1244,11 +1268,11 @@
       <c r="D22" s="4">
         <v>0</v>
       </c>
-      <c r="E22" s="12"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="14"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="18"/>
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C23" s="2" t="s">
@@ -1257,11 +1281,11 @@
       <c r="D23" s="4">
         <v>0</v>
       </c>
-      <c r="E23" s="12"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="14"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="18"/>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C24" s="2" t="s">
@@ -1270,11 +1294,11 @@
       <c r="D24" s="4">
         <v>0</v>
       </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="14"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="18"/>
     </row>
     <row r="25" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C25" s="2" t="s">
@@ -1283,11 +1307,11 @@
       <c r="D25" s="4">
         <v>0</v>
       </c>
-      <c r="E25" s="12"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="14"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="18"/>
     </row>
     <row r="26" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C26" s="2" t="s">
@@ -1296,11 +1320,11 @@
       <c r="D26" s="4">
         <v>0</v>
       </c>
-      <c r="E26" s="12"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="14"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="18"/>
     </row>
     <row r="27" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C27" s="2" t="s">
@@ -1309,11 +1333,11 @@
       <c r="D27" s="4">
         <v>0</v>
       </c>
-      <c r="E27" s="12"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="14"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="18"/>
     </row>
     <row r="28" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C28" s="2" t="s">
@@ -1322,11 +1346,11 @@
       <c r="D28" s="4">
         <v>0</v>
       </c>
-      <c r="E28" s="12"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="14"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="18"/>
     </row>
     <row r="29" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C29" s="2" t="s">
@@ -1335,11 +1359,11 @@
       <c r="D29" s="4">
         <v>0</v>
       </c>
-      <c r="E29" s="12"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="14"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="18"/>
     </row>
     <row r="30" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="9" t="s">
@@ -1347,402 +1371,414 @@
       </c>
       <c r="D30" s="8">
         <f>(D29+D28+D27+D26+D25+D24+D23+D22+D21+D20+D19+D18+D17+D16+D14+D15+D13+D12)/18</f>
-        <v>0</v>
-      </c>
-      <c r="E30" s="21"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="23"/>
+        <v>0.25</v>
+      </c>
+      <c r="E30" s="31"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="33"/>
     </row>
     <row r="31" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C31" s="27" t="s">
+      <c r="C31" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="28"/>
-      <c r="E31" s="15" t="s">
+      <c r="D31" s="23"/>
+      <c r="E31" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="17"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="35"/>
+      <c r="H31" s="35"/>
+      <c r="I31" s="36"/>
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C32" s="35" t="s">
+      <c r="C32" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="36">
-        <v>0.15</v>
-      </c>
-      <c r="E32" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="14"/>
+      <c r="D32" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="18"/>
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C33" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D33" s="36">
-        <v>0.15</v>
-      </c>
-      <c r="E33" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="14"/>
+      <c r="D33" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="18"/>
     </row>
     <row r="34" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C34" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D34" s="36">
-        <v>0.15</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="14"/>
+      <c r="D34" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="18"/>
     </row>
     <row r="35" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C35" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="36">
-        <v>0.15</v>
-      </c>
-      <c r="E35" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="14"/>
+      <c r="D35" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="18"/>
     </row>
     <row r="36" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C36" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D36" s="36">
-        <v>0.15</v>
-      </c>
-      <c r="E36" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="14"/>
+      <c r="D36" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="18"/>
     </row>
     <row r="37" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C37" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D37" s="36">
-        <v>0.15</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="14"/>
+      <c r="D37" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="18"/>
     </row>
     <row r="38" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C38" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D38" s="36">
-        <v>0.15</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="14"/>
+      <c r="D38" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="18"/>
     </row>
     <row r="39" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C39" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D39" s="36">
-        <v>0.15</v>
-      </c>
-      <c r="E39" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
-      <c r="I39" s="14"/>
+      <c r="D39" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="18"/>
     </row>
     <row r="40" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C40" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D40" s="36">
-        <v>0.15</v>
-      </c>
-      <c r="E40" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
-      <c r="I40" s="14"/>
+      <c r="D40" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="18"/>
     </row>
     <row r="41" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C41" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D41" s="36">
-        <v>0.15</v>
-      </c>
-      <c r="E41" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="14"/>
+      <c r="D41" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="18"/>
     </row>
     <row r="42" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C42" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D42" s="36">
-        <v>0.15</v>
-      </c>
-      <c r="E42" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="14"/>
+      <c r="D42" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="18"/>
     </row>
     <row r="43" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C43" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D43" s="36">
-        <v>0.15</v>
-      </c>
-      <c r="E43" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="13"/>
-      <c r="I43" s="14"/>
+      <c r="D43" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F43" s="17"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="18"/>
     </row>
     <row r="44" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C44" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D44" s="36">
-        <v>0.15</v>
-      </c>
-      <c r="E44" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
-      <c r="I44" s="14"/>
+      <c r="D44" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="17"/>
+      <c r="I44" s="18"/>
     </row>
     <row r="45" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C45" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D45" s="36">
-        <v>0.15</v>
-      </c>
-      <c r="E45" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="13"/>
-      <c r="I45" s="14"/>
+      <c r="D45" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="E45" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F45" s="17"/>
+      <c r="G45" s="17"/>
+      <c r="H45" s="17"/>
+      <c r="I45" s="18"/>
     </row>
     <row r="46" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C46" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D46" s="36">
-        <v>0.15</v>
-      </c>
-      <c r="E46" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="13"/>
-      <c r="I46" s="14"/>
+      <c r="D46" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="E46" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="18"/>
     </row>
     <row r="47" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C47" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D47" s="36">
-        <v>0.15</v>
-      </c>
-      <c r="E47" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13"/>
-      <c r="H47" s="13"/>
-      <c r="I47" s="14"/>
+      <c r="D47" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="E47" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="18"/>
     </row>
     <row r="48" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C48" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D48" s="36">
-        <v>0.15</v>
-      </c>
-      <c r="E48" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F48" s="13"/>
-      <c r="G48" s="13"/>
-      <c r="H48" s="13"/>
-      <c r="I48" s="14"/>
+      <c r="D48" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="E48" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="18"/>
     </row>
     <row r="49" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C49" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D49" s="36">
-        <v>0.15</v>
-      </c>
-      <c r="E49" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
-      <c r="H49" s="13"/>
-      <c r="I49" s="14"/>
+      <c r="D49" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="E49" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F49" s="17"/>
+      <c r="G49" s="17"/>
+      <c r="H49" s="17"/>
+      <c r="I49" s="18"/>
     </row>
     <row r="50" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C50" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D50" s="36">
-        <v>0.15</v>
-      </c>
-      <c r="E50" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
-      <c r="H50" s="13"/>
-      <c r="I50" s="14"/>
+      <c r="D50" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="E50" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
+      <c r="H50" s="17"/>
+      <c r="I50" s="18"/>
     </row>
     <row r="51" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C51" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D51" s="36">
-        <v>0.15</v>
-      </c>
-      <c r="E51" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F51" s="13"/>
-      <c r="G51" s="13"/>
-      <c r="H51" s="13"/>
-      <c r="I51" s="14"/>
+      <c r="D51" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="E51" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F51" s="17"/>
+      <c r="G51" s="17"/>
+      <c r="H51" s="17"/>
+      <c r="I51" s="18"/>
     </row>
     <row r="52" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C52" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D52" s="36">
-        <v>0.15</v>
-      </c>
-      <c r="E52" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F52" s="13"/>
-      <c r="G52" s="13"/>
-      <c r="H52" s="13"/>
-      <c r="I52" s="14"/>
+      <c r="D52" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="E52" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F52" s="17"/>
+      <c r="G52" s="17"/>
+      <c r="H52" s="17"/>
+      <c r="I52" s="18"/>
     </row>
     <row r="53" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C53" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D53" s="36">
-        <v>0.15</v>
-      </c>
-      <c r="E53" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F53" s="13"/>
-      <c r="G53" s="13"/>
-      <c r="H53" s="13"/>
-      <c r="I53" s="14"/>
+      <c r="D53" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="E53" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F53" s="17"/>
+      <c r="G53" s="17"/>
+      <c r="H53" s="17"/>
+      <c r="I53" s="18"/>
     </row>
     <row r="54" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C54" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D54" s="36">
-        <v>0.15</v>
-      </c>
-      <c r="E54" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F54" s="13"/>
-      <c r="G54" s="13"/>
-      <c r="H54" s="13"/>
-      <c r="I54" s="14"/>
+      <c r="D54" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="E54" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F54" s="17"/>
+      <c r="G54" s="17"/>
+      <c r="H54" s="17"/>
+      <c r="I54" s="18"/>
     </row>
     <row r="55" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C55" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D55" s="37">
+      <c r="D55" s="14">
         <f>(D41+D40+D39+D38+D37+D36+D35+D34+D33+D32+D42+D43+D44+D45+D46+D47+D48+D49+D50+D51+D52+D53+D54)/11</f>
         <v>0.31363636363636355</v>
       </c>
-      <c r="E55" s="38"/>
-      <c r="F55" s="38"/>
-      <c r="G55" s="38"/>
-      <c r="H55" s="38"/>
-      <c r="I55" s="39"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="E55:I55"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="E44:I44"/>
-    <mergeCell ref="E45:I45"/>
-    <mergeCell ref="E46:I46"/>
-    <mergeCell ref="E47:I47"/>
-    <mergeCell ref="E48:I48"/>
-    <mergeCell ref="E49:I49"/>
-    <mergeCell ref="E50:I50"/>
-    <mergeCell ref="E51:I51"/>
-    <mergeCell ref="E52:I52"/>
-    <mergeCell ref="E53:I53"/>
-    <mergeCell ref="E54:I54"/>
+    <mergeCell ref="E41:I41"/>
+    <mergeCell ref="E36:I36"/>
+    <mergeCell ref="E37:I37"/>
+    <mergeCell ref="E38:I38"/>
+    <mergeCell ref="E39:I39"/>
+    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="E31:I31"/>
+    <mergeCell ref="E32:I32"/>
+    <mergeCell ref="E33:I33"/>
+    <mergeCell ref="E34:I34"/>
+    <mergeCell ref="E35:I35"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="E28:I28"/>
+    <mergeCell ref="E29:I29"/>
+    <mergeCell ref="E30:I30"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="E19:I19"/>
+    <mergeCell ref="E20:I20"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C5:D5"/>
@@ -1759,32 +1795,20 @@
     <mergeCell ref="E13:I13"/>
     <mergeCell ref="E14:I14"/>
     <mergeCell ref="E15:I15"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="E17:I17"/>
-    <mergeCell ref="E18:I18"/>
-    <mergeCell ref="E19:I19"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="E25:I25"/>
-    <mergeCell ref="E26:I26"/>
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="E28:I28"/>
-    <mergeCell ref="E29:I29"/>
-    <mergeCell ref="E30:I30"/>
-    <mergeCell ref="E31:I31"/>
-    <mergeCell ref="E32:I32"/>
-    <mergeCell ref="E33:I33"/>
-    <mergeCell ref="E34:I34"/>
-    <mergeCell ref="E35:I35"/>
-    <mergeCell ref="E41:I41"/>
-    <mergeCell ref="E36:I36"/>
-    <mergeCell ref="E37:I37"/>
-    <mergeCell ref="E38:I38"/>
-    <mergeCell ref="E39:I39"/>
-    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="E55:I55"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="E44:I44"/>
+    <mergeCell ref="E45:I45"/>
+    <mergeCell ref="E46:I46"/>
+    <mergeCell ref="E47:I47"/>
+    <mergeCell ref="E48:I48"/>
+    <mergeCell ref="E49:I49"/>
+    <mergeCell ref="E50:I50"/>
+    <mergeCell ref="E51:I51"/>
+    <mergeCell ref="E52:I52"/>
+    <mergeCell ref="E53:I53"/>
+    <mergeCell ref="E54:I54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualizado a fecha 20 de marzo ya
</commit_message>
<xml_diff>
--- a/Cronograma-July-Tesis.xlsx
+++ b/Cronograma-July-Tesis.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="58">
   <si>
     <t>Cronograma</t>
   </si>
@@ -198,12 +198,6 @@
   </si>
   <si>
     <t>Falta revisar por Giovany y REFERENCIAR LA PARTE QUE DICE QUE EL CUIDADOR MUERE PRIMERO QUE EL PACIENTE</t>
-  </si>
-  <si>
-    <t>Revisar nuevamente</t>
-  </si>
-  <si>
-    <t>añadir los objetivos que faltan</t>
   </si>
 </sst>
 </file>
@@ -629,79 +623,79 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -986,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17:I17"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26:I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1002,10 +996,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="19"/>
+      <c r="D2" s="24"/>
     </row>
     <row r="3" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1015,26 +1009,26 @@
       <c r="D4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="26"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="31"/>
     </row>
     <row r="5" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="27" t="s">
+      <c r="D5" s="26"/>
+      <c r="E5" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="29"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="34"/>
     </row>
     <row r="6" spans="3:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="5" t="s">
@@ -1043,13 +1037,13 @@
       <c r="D6" s="6">
         <v>0.85</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="18"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="16"/>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
@@ -1058,11 +1052,11 @@
       <c r="D7" s="4">
         <v>0</v>
       </c>
-      <c r="E7" s="30"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="18"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="16"/>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
@@ -1071,13 +1065,13 @@
       <c r="D8" s="4">
         <v>0.9</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="18"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="16"/>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
@@ -1086,11 +1080,11 @@
       <c r="D9" s="4">
         <v>0</v>
       </c>
-      <c r="E9" s="30"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="18"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="16"/>
     </row>
     <row r="10" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="7" t="s">
@@ -1100,24 +1094,24 @@
         <f>(D9+D8+D7+D6)/4</f>
         <v>0.4375</v>
       </c>
-      <c r="E10" s="31"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="33"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="23"/>
     </row>
     <row r="11" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="34" t="s">
+      <c r="D11" s="26"/>
+      <c r="E11" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="36"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="19"/>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C12" s="5" t="s">
@@ -1126,13 +1120,13 @@
       <c r="D12" s="6">
         <v>0.9</v>
       </c>
-      <c r="E12" s="37" t="s">
+      <c r="E12" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="39"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="37"/>
     </row>
     <row r="13" spans="3:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
@@ -1141,13 +1135,13 @@
       <c r="D13" s="6">
         <v>0.9</v>
       </c>
-      <c r="E13" s="37" t="s">
+      <c r="E13" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="39"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="37"/>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
@@ -1156,13 +1150,13 @@
       <c r="D14" s="4">
         <v>0.9</v>
       </c>
-      <c r="E14" s="37" t="s">
+      <c r="E14" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="39"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="37"/>
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
@@ -1171,56 +1165,56 @@
       <c r="D15" s="4">
         <v>0.9</v>
       </c>
-      <c r="E15" s="37" t="s">
+      <c r="E15" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="39"/>
-    </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="37"/>
+    </row>
+    <row r="16" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="E16" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="18"/>
-    </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+        <v>0.9</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="37"/>
+    </row>
+    <row r="17" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="E17" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="18"/>
+        <v>0.9</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="37"/>
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="4">
-        <v>0</v>
-      </c>
-      <c r="E18" s="30"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="18"/>
+        <v>0.3</v>
+      </c>
+      <c r="E18" s="20"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="16"/>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
@@ -1229,11 +1223,11 @@
       <c r="D19" s="4">
         <v>0</v>
       </c>
-      <c r="E19" s="30"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="18"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="16"/>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C20" s="2" t="s">
@@ -1242,11 +1236,11 @@
       <c r="D20" s="4">
         <v>0</v>
       </c>
-      <c r="E20" s="30"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="18"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="16"/>
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C21" s="2" t="s">
@@ -1255,11 +1249,11 @@
       <c r="D21" s="4">
         <v>0</v>
       </c>
-      <c r="E21" s="30"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="18"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="16"/>
     </row>
     <row r="22" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C22" s="2" t="s">
@@ -1268,11 +1262,11 @@
       <c r="D22" s="4">
         <v>0</v>
       </c>
-      <c r="E22" s="30"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="18"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="16"/>
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C23" s="2" t="s">
@@ -1281,11 +1275,11 @@
       <c r="D23" s="4">
         <v>0</v>
       </c>
-      <c r="E23" s="30"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="18"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="16"/>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C24" s="2" t="s">
@@ -1294,11 +1288,11 @@
       <c r="D24" s="4">
         <v>0</v>
       </c>
-      <c r="E24" s="30"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="18"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="16"/>
     </row>
     <row r="25" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C25" s="2" t="s">
@@ -1307,11 +1301,11 @@
       <c r="D25" s="4">
         <v>0</v>
       </c>
-      <c r="E25" s="30"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="18"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="16"/>
     </row>
     <row r="26" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C26" s="2" t="s">
@@ -1320,11 +1314,11 @@
       <c r="D26" s="4">
         <v>0</v>
       </c>
-      <c r="E26" s="30"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="18"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="16"/>
     </row>
     <row r="27" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C27" s="2" t="s">
@@ -1333,11 +1327,11 @@
       <c r="D27" s="4">
         <v>0</v>
       </c>
-      <c r="E27" s="30"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="18"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="16"/>
     </row>
     <row r="28" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C28" s="2" t="s">
@@ -1346,11 +1340,11 @@
       <c r="D28" s="4">
         <v>0</v>
       </c>
-      <c r="E28" s="30"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="18"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="16"/>
     </row>
     <row r="29" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C29" s="2" t="s">
@@ -1359,11 +1353,11 @@
       <c r="D29" s="4">
         <v>0</v>
       </c>
-      <c r="E29" s="30"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="18"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="16"/>
     </row>
     <row r="30" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="9" t="s">
@@ -1371,26 +1365,26 @@
       </c>
       <c r="D30" s="8">
         <f>(D29+D28+D27+D26+D25+D24+D23+D22+D21+D20+D19+D18+D17+D16+D14+D15+D13+D12)/18</f>
-        <v>0.25</v>
-      </c>
-      <c r="E30" s="31"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="32"/>
-      <c r="H30" s="32"/>
-      <c r="I30" s="33"/>
+        <v>0.31666666666666665</v>
+      </c>
+      <c r="E30" s="21"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="23"/>
     </row>
     <row r="31" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="23"/>
-      <c r="E31" s="34" t="s">
+      <c r="D31" s="28"/>
+      <c r="E31" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F31" s="35"/>
-      <c r="G31" s="35"/>
-      <c r="H31" s="35"/>
-      <c r="I31" s="36"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="19"/>
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C32" s="12" t="s">
@@ -1399,13 +1393,13 @@
       <c r="D32" s="13">
         <v>0.15</v>
       </c>
-      <c r="E32" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="18"/>
+      <c r="E32" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="16"/>
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C33" s="1" t="s">
@@ -1414,13 +1408,13 @@
       <c r="D33" s="13">
         <v>0.15</v>
       </c>
-      <c r="E33" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="18"/>
+      <c r="E33" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="16"/>
     </row>
     <row r="34" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C34" s="1" t="s">
@@ -1429,13 +1423,13 @@
       <c r="D34" s="13">
         <v>0.15</v>
       </c>
-      <c r="E34" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="18"/>
+      <c r="E34" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="16"/>
     </row>
     <row r="35" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C35" s="1" t="s">
@@ -1444,13 +1438,13 @@
       <c r="D35" s="13">
         <v>0.15</v>
       </c>
-      <c r="E35" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="18"/>
+      <c r="E35" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="16"/>
     </row>
     <row r="36" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C36" s="1" t="s">
@@ -1459,13 +1453,13 @@
       <c r="D36" s="13">
         <v>0.15</v>
       </c>
-      <c r="E36" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="18"/>
+      <c r="E36" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="16"/>
     </row>
     <row r="37" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C37" s="1" t="s">
@@ -1474,13 +1468,13 @@
       <c r="D37" s="13">
         <v>0.15</v>
       </c>
-      <c r="E37" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="18"/>
+      <c r="E37" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="16"/>
     </row>
     <row r="38" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C38" s="1" t="s">
@@ -1489,13 +1483,13 @@
       <c r="D38" s="13">
         <v>0.15</v>
       </c>
-      <c r="E38" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="18"/>
+      <c r="E38" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="16"/>
     </row>
     <row r="39" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C39" s="1" t="s">
@@ -1504,13 +1498,13 @@
       <c r="D39" s="13">
         <v>0.15</v>
       </c>
-      <c r="E39" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F39" s="17"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="18"/>
+      <c r="E39" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="16"/>
     </row>
     <row r="40" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C40" s="1" t="s">
@@ -1519,13 +1513,13 @@
       <c r="D40" s="13">
         <v>0.15</v>
       </c>
-      <c r="E40" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17"/>
-      <c r="I40" s="18"/>
+      <c r="E40" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="16"/>
     </row>
     <row r="41" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C41" s="1" t="s">
@@ -1534,13 +1528,13 @@
       <c r="D41" s="13">
         <v>0.15</v>
       </c>
-      <c r="E41" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="17"/>
-      <c r="I41" s="18"/>
+      <c r="E41" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="16"/>
     </row>
     <row r="42" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C42" s="1" t="s">
@@ -1549,13 +1543,13 @@
       <c r="D42" s="13">
         <v>0.15</v>
       </c>
-      <c r="E42" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="17"/>
-      <c r="I42" s="18"/>
+      <c r="E42" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="16"/>
     </row>
     <row r="43" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C43" s="1" t="s">
@@ -1564,13 +1558,13 @@
       <c r="D43" s="13">
         <v>0.15</v>
       </c>
-      <c r="E43" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F43" s="17"/>
-      <c r="G43" s="17"/>
-      <c r="H43" s="17"/>
-      <c r="I43" s="18"/>
+      <c r="E43" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="16"/>
     </row>
     <row r="44" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C44" s="1" t="s">
@@ -1579,13 +1573,13 @@
       <c r="D44" s="13">
         <v>0.15</v>
       </c>
-      <c r="E44" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F44" s="17"/>
-      <c r="G44" s="17"/>
-      <c r="H44" s="17"/>
-      <c r="I44" s="18"/>
+      <c r="E44" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="16"/>
     </row>
     <row r="45" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C45" s="1" t="s">
@@ -1594,13 +1588,13 @@
       <c r="D45" s="13">
         <v>0.15</v>
       </c>
-      <c r="E45" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F45" s="17"/>
-      <c r="G45" s="17"/>
-      <c r="H45" s="17"/>
-      <c r="I45" s="18"/>
+      <c r="E45" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="16"/>
     </row>
     <row r="46" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C46" s="1" t="s">
@@ -1609,13 +1603,13 @@
       <c r="D46" s="13">
         <v>0.15</v>
       </c>
-      <c r="E46" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F46" s="17"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="17"/>
-      <c r="I46" s="18"/>
+      <c r="E46" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="16"/>
     </row>
     <row r="47" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C47" s="1" t="s">
@@ -1624,13 +1618,13 @@
       <c r="D47" s="13">
         <v>0.15</v>
       </c>
-      <c r="E47" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F47" s="17"/>
-      <c r="G47" s="17"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="18"/>
+      <c r="E47" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="16"/>
     </row>
     <row r="48" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C48" s="1" t="s">
@@ -1639,13 +1633,13 @@
       <c r="D48" s="13">
         <v>0.15</v>
       </c>
-      <c r="E48" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F48" s="17"/>
-      <c r="G48" s="17"/>
-      <c r="H48" s="17"/>
-      <c r="I48" s="18"/>
+      <c r="E48" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F48" s="15"/>
+      <c r="G48" s="15"/>
+      <c r="H48" s="15"/>
+      <c r="I48" s="16"/>
     </row>
     <row r="49" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C49" s="1" t="s">
@@ -1654,13 +1648,13 @@
       <c r="D49" s="13">
         <v>0.15</v>
       </c>
-      <c r="E49" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F49" s="17"/>
-      <c r="G49" s="17"/>
-      <c r="H49" s="17"/>
-      <c r="I49" s="18"/>
+      <c r="E49" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F49" s="15"/>
+      <c r="G49" s="15"/>
+      <c r="H49" s="15"/>
+      <c r="I49" s="16"/>
     </row>
     <row r="50" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C50" s="1" t="s">
@@ -1669,13 +1663,13 @@
       <c r="D50" s="13">
         <v>0.15</v>
       </c>
-      <c r="E50" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F50" s="17"/>
-      <c r="G50" s="17"/>
-      <c r="H50" s="17"/>
-      <c r="I50" s="18"/>
+      <c r="E50" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="15"/>
+      <c r="I50" s="16"/>
     </row>
     <row r="51" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C51" s="1" t="s">
@@ -1684,13 +1678,13 @@
       <c r="D51" s="13">
         <v>0.15</v>
       </c>
-      <c r="E51" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F51" s="17"/>
-      <c r="G51" s="17"/>
-      <c r="H51" s="17"/>
-      <c r="I51" s="18"/>
+      <c r="E51" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="15"/>
+      <c r="I51" s="16"/>
     </row>
     <row r="52" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C52" s="1" t="s">
@@ -1699,13 +1693,13 @@
       <c r="D52" s="13">
         <v>0.15</v>
       </c>
-      <c r="E52" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F52" s="17"/>
-      <c r="G52" s="17"/>
-      <c r="H52" s="17"/>
-      <c r="I52" s="18"/>
+      <c r="E52" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F52" s="15"/>
+      <c r="G52" s="15"/>
+      <c r="H52" s="15"/>
+      <c r="I52" s="16"/>
     </row>
     <row r="53" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C53" s="1" t="s">
@@ -1714,13 +1708,13 @@
       <c r="D53" s="13">
         <v>0.15</v>
       </c>
-      <c r="E53" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F53" s="17"/>
-      <c r="G53" s="17"/>
-      <c r="H53" s="17"/>
-      <c r="I53" s="18"/>
+      <c r="E53" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="15"/>
+      <c r="I53" s="16"/>
     </row>
     <row r="54" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C54" s="1" t="s">
@@ -1729,13 +1723,13 @@
       <c r="D54" s="13">
         <v>0.15</v>
       </c>
-      <c r="E54" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F54" s="17"/>
-      <c r="G54" s="17"/>
-      <c r="H54" s="17"/>
-      <c r="I54" s="18"/>
+      <c r="E54" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="16"/>
     </row>
     <row r="55" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C55" s="3" t="s">
@@ -1745,40 +1739,28 @@
         <f>(D41+D40+D39+D38+D37+D36+D35+D34+D33+D32+D42+D43+D44+D45+D46+D47+D48+D49+D50+D51+D52+D53+D54)/11</f>
         <v>0.31363636363636355</v>
       </c>
-      <c r="E55" s="15"/>
-      <c r="F55" s="15"/>
-      <c r="G55" s="15"/>
-      <c r="H55" s="15"/>
-      <c r="I55" s="16"/>
+      <c r="E55" s="38"/>
+      <c r="F55" s="38"/>
+      <c r="G55" s="38"/>
+      <c r="H55" s="38"/>
+      <c r="I55" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="E41:I41"/>
-    <mergeCell ref="E36:I36"/>
-    <mergeCell ref="E37:I37"/>
-    <mergeCell ref="E38:I38"/>
-    <mergeCell ref="E39:I39"/>
-    <mergeCell ref="E40:I40"/>
-    <mergeCell ref="E31:I31"/>
-    <mergeCell ref="E32:I32"/>
-    <mergeCell ref="E33:I33"/>
-    <mergeCell ref="E34:I34"/>
-    <mergeCell ref="E35:I35"/>
-    <mergeCell ref="E26:I26"/>
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="E28:I28"/>
-    <mergeCell ref="E29:I29"/>
-    <mergeCell ref="E30:I30"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="E25:I25"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="E17:I17"/>
-    <mergeCell ref="E18:I18"/>
-    <mergeCell ref="E19:I19"/>
-    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="E55:I55"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="E44:I44"/>
+    <mergeCell ref="E45:I45"/>
+    <mergeCell ref="E46:I46"/>
+    <mergeCell ref="E47:I47"/>
+    <mergeCell ref="E48:I48"/>
+    <mergeCell ref="E49:I49"/>
+    <mergeCell ref="E50:I50"/>
+    <mergeCell ref="E51:I51"/>
+    <mergeCell ref="E52:I52"/>
+    <mergeCell ref="E53:I53"/>
+    <mergeCell ref="E54:I54"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C5:D5"/>
@@ -1795,20 +1777,32 @@
     <mergeCell ref="E13:I13"/>
     <mergeCell ref="E14:I14"/>
     <mergeCell ref="E15:I15"/>
-    <mergeCell ref="E55:I55"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="E44:I44"/>
-    <mergeCell ref="E45:I45"/>
-    <mergeCell ref="E46:I46"/>
-    <mergeCell ref="E47:I47"/>
-    <mergeCell ref="E48:I48"/>
-    <mergeCell ref="E49:I49"/>
-    <mergeCell ref="E50:I50"/>
-    <mergeCell ref="E51:I51"/>
-    <mergeCell ref="E52:I52"/>
-    <mergeCell ref="E53:I53"/>
-    <mergeCell ref="E54:I54"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="E19:I19"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="E28:I28"/>
+    <mergeCell ref="E29:I29"/>
+    <mergeCell ref="E30:I30"/>
+    <mergeCell ref="E31:I31"/>
+    <mergeCell ref="E32:I32"/>
+    <mergeCell ref="E33:I33"/>
+    <mergeCell ref="E34:I34"/>
+    <mergeCell ref="E35:I35"/>
+    <mergeCell ref="E41:I41"/>
+    <mergeCell ref="E36:I36"/>
+    <mergeCell ref="E37:I37"/>
+    <mergeCell ref="E38:I38"/>
+    <mergeCell ref="E39:I39"/>
+    <mergeCell ref="E40:I40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualizado a Fecha 23 de marzo Actualizado
</commit_message>
<xml_diff>
--- a/Cronograma-July-Tesis.xlsx
+++ b/Cronograma-July-Tesis.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="59">
   <si>
     <t>Cronograma</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>Falta revisar por Giovany y REFERENCIAR LA PARTE QUE DICE QUE EL CUIDADOR MUERE PRIMERO QUE EL PACIENTE</t>
+  </si>
+  <si>
+    <t>revisar nuevamente</t>
   </si>
 </sst>
 </file>
@@ -623,12 +626,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -638,51 +692,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -690,12 +699,6 @@
       <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -980,8 +983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26:I26"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27:I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -996,10 +999,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="24"/>
+      <c r="D2" s="19"/>
     </row>
     <row r="3" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1009,26 +1012,26 @@
       <c r="D4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="31"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="26"/>
     </row>
     <row r="5" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="32" t="s">
+      <c r="D5" s="21"/>
+      <c r="E5" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="34"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="29"/>
     </row>
     <row r="6" spans="3:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="5" t="s">
@@ -1037,13 +1040,13 @@
       <c r="D6" s="6">
         <v>0.85</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="16"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="18"/>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
@@ -1052,11 +1055,11 @@
       <c r="D7" s="4">
         <v>0</v>
       </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="16"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="18"/>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
@@ -1065,13 +1068,13 @@
       <c r="D8" s="4">
         <v>0.9</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="16"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="18"/>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
@@ -1080,11 +1083,11 @@
       <c r="D9" s="4">
         <v>0</v>
       </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="16"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="18"/>
     </row>
     <row r="10" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="7" t="s">
@@ -1094,24 +1097,24 @@
         <f>(D9+D8+D7+D6)/4</f>
         <v>0.4375</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="23"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="33"/>
     </row>
     <row r="11" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="17" t="s">
+      <c r="D11" s="21"/>
+      <c r="E11" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="19"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="36"/>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C12" s="5" t="s">
@@ -1120,13 +1123,13 @@
       <c r="D12" s="6">
         <v>0.9</v>
       </c>
-      <c r="E12" s="35" t="s">
+      <c r="E12" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="37"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="39"/>
     </row>
     <row r="13" spans="3:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
@@ -1135,13 +1138,13 @@
       <c r="D13" s="6">
         <v>0.9</v>
       </c>
-      <c r="E13" s="35" t="s">
+      <c r="E13" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="37"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="39"/>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
@@ -1150,13 +1153,13 @@
       <c r="D14" s="4">
         <v>0.9</v>
       </c>
-      <c r="E14" s="35" t="s">
+      <c r="E14" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="37"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="39"/>
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
@@ -1165,13 +1168,13 @@
       <c r="D15" s="4">
         <v>0.9</v>
       </c>
-      <c r="E15" s="35" t="s">
+      <c r="E15" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="37"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="39"/>
     </row>
     <row r="16" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
@@ -1180,13 +1183,13 @@
       <c r="D16" s="4">
         <v>0.9</v>
       </c>
-      <c r="E16" s="35" t="s">
+      <c r="E16" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="37"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="39"/>
     </row>
     <row r="17" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
@@ -1195,143 +1198,163 @@
       <c r="D17" s="4">
         <v>0.9</v>
       </c>
-      <c r="E17" s="35" t="s">
+      <c r="E17" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="37"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="39"/>
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="E18" s="20"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="16"/>
+        <v>0.8</v>
+      </c>
+      <c r="E18" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="18"/>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D19" s="4">
-        <v>0</v>
-      </c>
-      <c r="E19" s="20"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="16"/>
+        <v>0.4</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="18"/>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C20" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D20" s="4">
-        <v>0</v>
-      </c>
-      <c r="E20" s="20"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="16"/>
+        <v>0.4</v>
+      </c>
+      <c r="E20" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="18"/>
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C21" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D21" s="4">
-        <v>0</v>
-      </c>
-      <c r="E21" s="20"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="16"/>
+        <v>0.3</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="18"/>
     </row>
     <row r="22" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C22" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D22" s="4">
-        <v>0</v>
-      </c>
-      <c r="E22" s="20"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="16"/>
+        <v>0.5</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="18"/>
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C23" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D23" s="4">
-        <v>0</v>
-      </c>
-      <c r="E23" s="20"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="16"/>
+        <v>0.4</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="18"/>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C24" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D24" s="4">
-        <v>0</v>
-      </c>
-      <c r="E24" s="20"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="16"/>
+        <v>0.5</v>
+      </c>
+      <c r="E24" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="18"/>
     </row>
     <row r="25" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C25" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D25" s="4">
-        <v>0</v>
-      </c>
-      <c r="E25" s="20"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="16"/>
+        <v>0.5</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="18"/>
     </row>
     <row r="26" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C26" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D26" s="4">
-        <v>0</v>
-      </c>
-      <c r="E26" s="20"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="16"/>
+        <v>0.5</v>
+      </c>
+      <c r="E26" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="18"/>
     </row>
     <row r="27" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C27" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D27" s="4">
-        <v>0</v>
-      </c>
-      <c r="E27" s="20"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="16"/>
+        <v>0.5</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="18"/>
     </row>
     <row r="28" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C28" s="2" t="s">
@@ -1340,24 +1363,28 @@
       <c r="D28" s="4">
         <v>0</v>
       </c>
-      <c r="E28" s="20"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="16"/>
+      <c r="E28" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="18"/>
     </row>
     <row r="29" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C29" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D29" s="4">
-        <v>0</v>
-      </c>
-      <c r="E29" s="20"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="16"/>
+        <v>0.5</v>
+      </c>
+      <c r="E29" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="18"/>
     </row>
     <row r="30" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="9" t="s">
@@ -1365,26 +1392,26 @@
       </c>
       <c r="D30" s="8">
         <f>(D29+D28+D27+D26+D25+D24+D23+D22+D21+D20+D19+D18+D17+D16+D14+D15+D13+D12)/18</f>
-        <v>0.31666666666666665</v>
-      </c>
-      <c r="E30" s="21"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="23"/>
+        <v>0.59444444444444455</v>
+      </c>
+      <c r="E30" s="31"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="33"/>
     </row>
     <row r="31" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C31" s="27" t="s">
+      <c r="C31" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="28"/>
-      <c r="E31" s="17" t="s">
+      <c r="D31" s="23"/>
+      <c r="E31" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="19"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="35"/>
+      <c r="H31" s="35"/>
+      <c r="I31" s="36"/>
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C32" s="12" t="s">
@@ -1393,13 +1420,13 @@
       <c r="D32" s="13">
         <v>0.15</v>
       </c>
-      <c r="E32" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="16"/>
+      <c r="E32" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="18"/>
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C33" s="1" t="s">
@@ -1408,13 +1435,13 @@
       <c r="D33" s="13">
         <v>0.15</v>
       </c>
-      <c r="E33" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="16"/>
+      <c r="E33" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="18"/>
     </row>
     <row r="34" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C34" s="1" t="s">
@@ -1423,13 +1450,13 @@
       <c r="D34" s="13">
         <v>0.15</v>
       </c>
-      <c r="E34" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="16"/>
+      <c r="E34" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="18"/>
     </row>
     <row r="35" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C35" s="1" t="s">
@@ -1438,13 +1465,13 @@
       <c r="D35" s="13">
         <v>0.15</v>
       </c>
-      <c r="E35" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="16"/>
+      <c r="E35" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="18"/>
     </row>
     <row r="36" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C36" s="1" t="s">
@@ -1453,13 +1480,13 @@
       <c r="D36" s="13">
         <v>0.15</v>
       </c>
-      <c r="E36" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="16"/>
+      <c r="E36" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="18"/>
     </row>
     <row r="37" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C37" s="1" t="s">
@@ -1468,13 +1495,13 @@
       <c r="D37" s="13">
         <v>0.15</v>
       </c>
-      <c r="E37" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="16"/>
+      <c r="E37" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="18"/>
     </row>
     <row r="38" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C38" s="1" t="s">
@@ -1483,13 +1510,13 @@
       <c r="D38" s="13">
         <v>0.15</v>
       </c>
-      <c r="E38" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="16"/>
+      <c r="E38" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="18"/>
     </row>
     <row r="39" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C39" s="1" t="s">
@@ -1498,13 +1525,13 @@
       <c r="D39" s="13">
         <v>0.15</v>
       </c>
-      <c r="E39" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F39" s="15"/>
-      <c r="G39" s="15"/>
-      <c r="H39" s="15"/>
-      <c r="I39" s="16"/>
+      <c r="E39" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="18"/>
     </row>
     <row r="40" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C40" s="1" t="s">
@@ -1513,13 +1540,13 @@
       <c r="D40" s="13">
         <v>0.15</v>
       </c>
-      <c r="E40" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F40" s="15"/>
-      <c r="G40" s="15"/>
-      <c r="H40" s="15"/>
-      <c r="I40" s="16"/>
+      <c r="E40" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="18"/>
     </row>
     <row r="41" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C41" s="1" t="s">
@@ -1528,13 +1555,13 @@
       <c r="D41" s="13">
         <v>0.15</v>
       </c>
-      <c r="E41" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
-      <c r="H41" s="15"/>
-      <c r="I41" s="16"/>
+      <c r="E41" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="18"/>
     </row>
     <row r="42" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C42" s="1" t="s">
@@ -1543,13 +1570,13 @@
       <c r="D42" s="13">
         <v>0.15</v>
       </c>
-      <c r="E42" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F42" s="15"/>
-      <c r="G42" s="15"/>
-      <c r="H42" s="15"/>
-      <c r="I42" s="16"/>
+      <c r="E42" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="18"/>
     </row>
     <row r="43" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C43" s="1" t="s">
@@ -1558,13 +1585,13 @@
       <c r="D43" s="13">
         <v>0.15</v>
       </c>
-      <c r="E43" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F43" s="15"/>
-      <c r="G43" s="15"/>
-      <c r="H43" s="15"/>
-      <c r="I43" s="16"/>
+      <c r="E43" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F43" s="17"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="18"/>
     </row>
     <row r="44" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C44" s="1" t="s">
@@ -1573,13 +1600,13 @@
       <c r="D44" s="13">
         <v>0.15</v>
       </c>
-      <c r="E44" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F44" s="15"/>
-      <c r="G44" s="15"/>
-      <c r="H44" s="15"/>
-      <c r="I44" s="16"/>
+      <c r="E44" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="17"/>
+      <c r="I44" s="18"/>
     </row>
     <row r="45" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C45" s="1" t="s">
@@ -1588,13 +1615,13 @@
       <c r="D45" s="13">
         <v>0.15</v>
       </c>
-      <c r="E45" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
-      <c r="H45" s="15"/>
-      <c r="I45" s="16"/>
+      <c r="E45" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F45" s="17"/>
+      <c r="G45" s="17"/>
+      <c r="H45" s="17"/>
+      <c r="I45" s="18"/>
     </row>
     <row r="46" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C46" s="1" t="s">
@@ -1603,13 +1630,13 @@
       <c r="D46" s="13">
         <v>0.15</v>
       </c>
-      <c r="E46" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F46" s="15"/>
-      <c r="G46" s="15"/>
-      <c r="H46" s="15"/>
-      <c r="I46" s="16"/>
+      <c r="E46" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="18"/>
     </row>
     <row r="47" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C47" s="1" t="s">
@@ -1618,13 +1645,13 @@
       <c r="D47" s="13">
         <v>0.15</v>
       </c>
-      <c r="E47" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F47" s="15"/>
-      <c r="G47" s="15"/>
-      <c r="H47" s="15"/>
-      <c r="I47" s="16"/>
+      <c r="E47" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="18"/>
     </row>
     <row r="48" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C48" s="1" t="s">
@@ -1633,13 +1660,13 @@
       <c r="D48" s="13">
         <v>0.15</v>
       </c>
-      <c r="E48" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F48" s="15"/>
-      <c r="G48" s="15"/>
-      <c r="H48" s="15"/>
-      <c r="I48" s="16"/>
+      <c r="E48" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="18"/>
     </row>
     <row r="49" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C49" s="1" t="s">
@@ -1648,13 +1675,13 @@
       <c r="D49" s="13">
         <v>0.15</v>
       </c>
-      <c r="E49" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F49" s="15"/>
-      <c r="G49" s="15"/>
-      <c r="H49" s="15"/>
-      <c r="I49" s="16"/>
+      <c r="E49" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F49" s="17"/>
+      <c r="G49" s="17"/>
+      <c r="H49" s="17"/>
+      <c r="I49" s="18"/>
     </row>
     <row r="50" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C50" s="1" t="s">
@@ -1663,13 +1690,13 @@
       <c r="D50" s="13">
         <v>0.15</v>
       </c>
-      <c r="E50" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F50" s="15"/>
-      <c r="G50" s="15"/>
-      <c r="H50" s="15"/>
-      <c r="I50" s="16"/>
+      <c r="E50" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
+      <c r="H50" s="17"/>
+      <c r="I50" s="18"/>
     </row>
     <row r="51" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C51" s="1" t="s">
@@ -1678,13 +1705,13 @@
       <c r="D51" s="13">
         <v>0.15</v>
       </c>
-      <c r="E51" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F51" s="15"/>
-      <c r="G51" s="15"/>
-      <c r="H51" s="15"/>
-      <c r="I51" s="16"/>
+      <c r="E51" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F51" s="17"/>
+      <c r="G51" s="17"/>
+      <c r="H51" s="17"/>
+      <c r="I51" s="18"/>
     </row>
     <row r="52" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C52" s="1" t="s">
@@ -1693,13 +1720,13 @@
       <c r="D52" s="13">
         <v>0.15</v>
       </c>
-      <c r="E52" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F52" s="15"/>
-      <c r="G52" s="15"/>
-      <c r="H52" s="15"/>
-      <c r="I52" s="16"/>
+      <c r="E52" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F52" s="17"/>
+      <c r="G52" s="17"/>
+      <c r="H52" s="17"/>
+      <c r="I52" s="18"/>
     </row>
     <row r="53" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C53" s="1" t="s">
@@ -1708,13 +1735,13 @@
       <c r="D53" s="13">
         <v>0.15</v>
       </c>
-      <c r="E53" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F53" s="15"/>
-      <c r="G53" s="15"/>
-      <c r="H53" s="15"/>
-      <c r="I53" s="16"/>
+      <c r="E53" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F53" s="17"/>
+      <c r="G53" s="17"/>
+      <c r="H53" s="17"/>
+      <c r="I53" s="18"/>
     </row>
     <row r="54" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C54" s="1" t="s">
@@ -1723,13 +1750,13 @@
       <c r="D54" s="13">
         <v>0.15</v>
       </c>
-      <c r="E54" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F54" s="15"/>
-      <c r="G54" s="15"/>
-      <c r="H54" s="15"/>
-      <c r="I54" s="16"/>
+      <c r="E54" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F54" s="17"/>
+      <c r="G54" s="17"/>
+      <c r="H54" s="17"/>
+      <c r="I54" s="18"/>
     </row>
     <row r="55" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C55" s="3" t="s">
@@ -1739,28 +1766,40 @@
         <f>(D41+D40+D39+D38+D37+D36+D35+D34+D33+D32+D42+D43+D44+D45+D46+D47+D48+D49+D50+D51+D52+D53+D54)/11</f>
         <v>0.31363636363636355</v>
       </c>
-      <c r="E55" s="38"/>
-      <c r="F55" s="38"/>
-      <c r="G55" s="38"/>
-      <c r="H55" s="38"/>
-      <c r="I55" s="39"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="E55:I55"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="E44:I44"/>
-    <mergeCell ref="E45:I45"/>
-    <mergeCell ref="E46:I46"/>
-    <mergeCell ref="E47:I47"/>
-    <mergeCell ref="E48:I48"/>
-    <mergeCell ref="E49:I49"/>
-    <mergeCell ref="E50:I50"/>
-    <mergeCell ref="E51:I51"/>
-    <mergeCell ref="E52:I52"/>
-    <mergeCell ref="E53:I53"/>
-    <mergeCell ref="E54:I54"/>
+    <mergeCell ref="E41:I41"/>
+    <mergeCell ref="E36:I36"/>
+    <mergeCell ref="E37:I37"/>
+    <mergeCell ref="E38:I38"/>
+    <mergeCell ref="E39:I39"/>
+    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="E31:I31"/>
+    <mergeCell ref="E32:I32"/>
+    <mergeCell ref="E33:I33"/>
+    <mergeCell ref="E34:I34"/>
+    <mergeCell ref="E35:I35"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="E28:I28"/>
+    <mergeCell ref="E29:I29"/>
+    <mergeCell ref="E30:I30"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="E19:I19"/>
+    <mergeCell ref="E20:I20"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C5:D5"/>
@@ -1777,32 +1816,20 @@
     <mergeCell ref="E13:I13"/>
     <mergeCell ref="E14:I14"/>
     <mergeCell ref="E15:I15"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="E17:I17"/>
-    <mergeCell ref="E18:I18"/>
-    <mergeCell ref="E19:I19"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="E25:I25"/>
-    <mergeCell ref="E26:I26"/>
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="E28:I28"/>
-    <mergeCell ref="E29:I29"/>
-    <mergeCell ref="E30:I30"/>
-    <mergeCell ref="E31:I31"/>
-    <mergeCell ref="E32:I32"/>
-    <mergeCell ref="E33:I33"/>
-    <mergeCell ref="E34:I34"/>
-    <mergeCell ref="E35:I35"/>
-    <mergeCell ref="E41:I41"/>
-    <mergeCell ref="E36:I36"/>
-    <mergeCell ref="E37:I37"/>
-    <mergeCell ref="E38:I38"/>
-    <mergeCell ref="E39:I39"/>
-    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="E55:I55"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="E44:I44"/>
+    <mergeCell ref="E45:I45"/>
+    <mergeCell ref="E46:I46"/>
+    <mergeCell ref="E47:I47"/>
+    <mergeCell ref="E48:I48"/>
+    <mergeCell ref="E49:I49"/>
+    <mergeCell ref="E50:I50"/>
+    <mergeCell ref="E51:I51"/>
+    <mergeCell ref="E52:I52"/>
+    <mergeCell ref="E53:I53"/>
+    <mergeCell ref="E54:I54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>